<commit_message>
Atualização agendada das bases de dados
</commit_message>
<xml_diff>
--- a/Data/g13.6.xlsx
+++ b/Data/g13.6.xlsx
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>6.3</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="4">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>12.2</v>
+        <v>12.1</v>
       </c>
     </row>
     <row r="7">
@@ -952,7 +952,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>10.4</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="27">
@@ -972,7 +972,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>8.6</v>
+        <v>8.699999999999999</v>
       </c>
     </row>
     <row r="28">
@@ -1032,7 +1032,7 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>9</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="31">
@@ -1092,7 +1092,7 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>13.6</v>
+        <v>13.7</v>
       </c>
     </row>
     <row r="34">
@@ -1132,7 +1132,7 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>15</v>
+        <v>15.1</v>
       </c>
     </row>
     <row r="36">
@@ -1192,7 +1192,7 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>11.9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39">
@@ -1212,7 +1212,7 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>11.2</v>
+        <v>11.3</v>
       </c>
     </row>
     <row r="40">

</xml_diff>